<commit_message>
#6 - Data opslaan
</commit_message>
<xml_diff>
--- a/outputs/maxaro.xlsx
+++ b/outputs/maxaro.xlsx
@@ -493,18 +493,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SW161911</t>
+          <t>SW108325</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>VSA61</t>
+          <t>M45-0600-43080</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Half Vrijstaand Bad Marano 170x80cm Acryl Glans Wit</t>
+          <t>Ronde badkamerspiegel met LED Verlichting 60cm</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -515,39 +515,39 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>baden</t>
+          <t>badkamerspiegels</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>half-vrijstaande-baden</t>
+          <t>badkamerspiegels-met-verlichting</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1045</v>
+        <v>219</v>
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/baden/half-vrijstaande-baden/half-vrijstaand-bad-marano-170x80cm-acryl-glans-wit-6682/</t>
+          <t>https://www.maxaro.nl/badkamerspiegels/badkamerspiegels-met-verlichting/ronde-badkamerspiegel-met-led-verlichting-60cm-6553/</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SW161922</t>
+          <t>SW161911</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>M45-1000-43080</t>
+          <t>VSA61</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Ronde badkamerspiegel met LED Verlichting 100cm</t>
+          <t>Half Vrijstaand Bad Marano 170x80cm Acryl Glans Wit</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -558,21 +558,21 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>badkamerspiegels</t>
+          <t>baden</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>badkamerspiegels-met-verlichting</t>
+          <t>half-vrijstaande-baden</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>329</v>
+        <v>1045</v>
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/badkamerspiegels/badkamerspiegels-met-verlichting/ronde-badkamerspiegel-met-led-verlichting-100cm-6555/</t>
+          <t>https://www.maxaro.nl/baden/half-vrijstaande-baden/half-vrijstaand-bad-marano-170x80cm-acryl-glans-wit-6682/</t>
         </is>
       </c>
     </row>
@@ -622,18 +622,18 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SW238204</t>
+          <t>SW1009</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>IPA12305M</t>
+          <t>GW-09013</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 120cm Zwarte Strepen Veiligheidsglas 8mm Mat Zwart</t>
+          <t>Douchewand Inloopdouche 90cm Veiligheidsglas 6 mm Chroom</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -653,30 +653,30 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>425</v>
+        <v>150</v>
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-120cm-zwarte-strepen-veiligheidsglas-8mm-mat-zwart-11190/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-90cm-veiligheidsglas-6-mm-chroom-81034/</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SW225871</t>
+          <t>SW161922</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>VSA72</t>
+          <t>M45-1000-43080</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Halfvrijstaand Bad Velino 180x80cm Acryl Glans Wit</t>
+          <t>Ronde badkamerspiegel met LED Verlichting 100cm</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -687,39 +687,39 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>baden</t>
+          <t>badkamerspiegels</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>half-vrijstaande-baden</t>
+          <t>badkamerspiegels-met-verlichting</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1045</v>
+        <v>329</v>
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/baden/half-vrijstaande-baden/halfvrijstaand-bad-velino-180x80cm-acryl-glans-wit-81175/</t>
+          <t>https://www.maxaro.nl/badkamerspiegels/badkamerspiegels-met-verlichting/ronde-badkamerspiegel-met-led-verlichting-100cm-6555/</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SW108325</t>
+          <t>SW161775</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>M45-0600-43080</t>
+          <t>DSC-0404-00000</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Ronde badkamerspiegel met LED Verlichting 60cm</t>
+          <t>Regendoucheset Easy Chrome, Thermostaatkraan, 22cm Hoofddouche, Chroom</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -730,39 +730,39 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>badkamerspiegels</t>
+          <t>kranen</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>badkamerspiegels-met-verlichting</t>
+          <t>regendouches</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/badkamerspiegels/badkamerspiegels-met-verlichting/ronde-badkamerspiegel-met-led-verlichting-60cm-6553/</t>
+          <t>https://www.maxaro.nl/kranen/regendouches/regendoucheset-easy-chrome-thermostaatkraan-22cm-hoofddouche-chroom-82903/</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SW161775</t>
+          <t>SW208804</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>DSC-0404-00000</t>
+          <t>GW-12013</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Regendoucheset Easy Chrome, Thermostaatkraan, 22cm Hoofddouche, Chroom</t>
+          <t>Douchewand Inloopdouche 120cm Veiligheidsglas 6 mm Chroom</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -773,21 +773,21 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>kranen</t>
+          <t>douches</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>regendouches</t>
+          <t>inloopdouches</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/kranen/regendouches/regendoucheset-easy-chrome-thermostaatkraan-22cm-hoofddouche-chroom-82903/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-120cm-veiligheidsglas-6-mm-chroom-82443/</t>
         </is>
       </c>
     </row>
@@ -837,18 +837,18 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>SW1008</t>
+          <t>SW225871</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>GW-10013</t>
+          <t>VSA72</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 100cm Veiligheidsglas 6 mm Chroom</t>
+          <t>Halfvrijstaand Bad Velino 180x80cm Acryl Glans Wit</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -859,39 +859,39 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>douches</t>
+          <t>baden</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>inloopdouches</t>
+          <t>half-vrijstaande-baden</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>160</v>
+        <v>1045</v>
       </c>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-100cm-veiligheidsglas-6-mm-chroom-81035/</t>
+          <t>https://www.maxaro.nl/baden/half-vrijstaande-baden/halfvrijstaand-bad-velino-180x80cm-acryl-glans-wit-81175/</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SW1009</t>
+          <t>SW238214</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>GW-09013</t>
+          <t>M10-1200-40500</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 90cm Veiligheidsglas 6 mm Chroom</t>
+          <t>Badkamerspiegel met LED Verlichting Lumo 120x60cm</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -902,39 +902,39 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>douches</t>
+          <t>badkamerspiegels</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>inloopdouches</t>
+          <t>badkamerspiegels-met-verlichting</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>150</v>
+        <v>259</v>
       </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-90cm-veiligheidsglas-6-mm-chroom-81034/</t>
+          <t>https://www.maxaro.nl/badkamerspiegels/badkamerspiegels-met-verlichting/badkamerspiegel-met-led-verlichting-lumo-120x60cm-6504/</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>SW157891</t>
+          <t>SW238204</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>XZ03-1880G</t>
+          <t>IPA12305M</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Ligbad Capri 180x80cm Acryl Glans Wit</t>
+          <t>Douchewand Inloopdouche 120cm Zwarte Strepen Veiligheidsglas 8mm Mat Zwart</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -945,39 +945,39 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>baden</t>
+          <t>douches</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>ligbaden</t>
+          <t>inloopdouches</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>229</v>
+        <v>425</v>
       </c>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/baden/ligbaden/ligbad-capri-180x80cm-acryl-glans-wit-6661/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-120cm-zwarte-strepen-veiligheidsglas-8mm-mat-zwart-11190/</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>SW238214</t>
+          <t>SW157891</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>M10-1200-40500</t>
+          <t>XZ03-1880G</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Badkamerspiegel met LED Verlichting Lumo 120x60cm</t>
+          <t>Ligbad Capri 180x80cm Acryl Glans Wit</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -988,39 +988,39 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>badkamerspiegels</t>
+          <t>baden</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>badkamerspiegels-met-verlichting</t>
+          <t>ligbaden</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>259</v>
+        <v>229</v>
       </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/badkamerspiegels/badkamerspiegels-met-verlichting/badkamerspiegel-met-led-verlichting-lumo-120x60cm-6504/</t>
+          <t>https://www.maxaro.nl/baden/ligbaden/ligbad-capri-180x80cm-acryl-glans-wit-6661/</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>SW208804</t>
+          <t>SW1008</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>GW-12013</t>
+          <t>GW-10013</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 120cm Veiligheidsglas 6 mm Chroom</t>
+          <t>Douchewand Inloopdouche 100cm Veiligheidsglas 6 mm Chroom</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1040,12 +1040,12 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-120cm-veiligheidsglas-6-mm-chroom-82443/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-100cm-veiligheidsglas-6-mm-chroom-81035/</t>
         </is>
       </c>
     </row>
@@ -1095,18 +1095,18 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>sw6328</t>
+          <t>SW1125</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>IPA10305M</t>
+          <t>IPA09305M</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 100cm Zwarte Strepen Veiligheidsglas 8mm Mat Zwart</t>
+          <t>Douchewand Inloopdouche 90cm Zwarte Strepen Veiligheidsglas 8mm Mat Zwart</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1126,30 +1126,30 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-100cm-zwarte-strepen-veiligheidsglas-8mm-mat-zwart-11157/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-90cm-zwarte-strepen-veiligheidsglas-8mm-mat-zwart-11123/</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>SW23914</t>
+          <t>SW108326</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>S0820-1000C</t>
+          <t>XZ02-1775G</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Douchewand met Schuifdeur Ruby Allure 100cm Chroom</t>
+          <t>Ligbad Piana 170x75cm Acryl Glans Wit</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1160,39 +1160,39 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>douches</t>
+          <t>baden</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>douchedeuren</t>
+          <t>ligbaden</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>300</v>
+        <v>199</v>
       </c>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchedeuren/douchewand-met-schuifdeur-ruby-allure-100cm-chroom-12608/</t>
+          <t>https://www.maxaro.nl/baden/ligbaden/ligbad-piana-170x75cm-acryl-glans-wit-6656/</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>SW238202</t>
+          <t>sw6328</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>S0820-1100C</t>
+          <t>IPA10305M</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Douchewand met Schuifdeur Ruby Allure 110cm Chroom</t>
+          <t>Douchewand Inloopdouche 100cm Zwarte Strepen Veiligheidsglas 8mm Mat Zwart</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1208,34 +1208,34 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>douchedeuren</t>
+          <t>inloopdouches</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>310</v>
+        <v>405</v>
       </c>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchedeuren/douchewand-met-schuifdeur-ruby-allure-110cm-chroom-12610/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-100cm-zwarte-strepen-veiligheidsglas-8mm-mat-zwart-11157/</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SW108326</t>
+          <t>SW238202</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>XZ02-1775G</t>
+          <t>S0820-1100C</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Ligbad Piana 170x75cm Acryl Glans Wit</t>
+          <t>Douchewand met Schuifdeur Ruby Allure 110cm Chroom</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1246,39 +1246,39 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>baden</t>
+          <t>douches</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>ligbaden</t>
+          <t>douchedeuren</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>199</v>
+        <v>310</v>
       </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/baden/ligbaden/ligbad-piana-170x75cm-acryl-glans-wit-6656/</t>
+          <t>https://www.maxaro.nl/douches/douchedeuren/douchewand-met-schuifdeur-ruby-allure-110cm-chroom-12610/</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>SW1125</t>
+          <t>SW23914</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>IPA09305M</t>
+          <t>S0820-1000C</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 90cm Zwarte Strepen Veiligheidsglas 8mm Mat Zwart</t>
+          <t>Douchewand met Schuifdeur Ruby Allure 100cm Chroom</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1294,34 +1294,34 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>inloopdouches</t>
+          <t>douchedeuren</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>395</v>
+        <v>300</v>
       </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-90cm-zwarte-strepen-veiligheidsglas-8mm-mat-zwart-11123/</t>
+          <t>https://www.maxaro.nl/douches/douchedeuren/douchewand-met-schuifdeur-ruby-allure-100cm-chroom-12608/</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>SW238201</t>
+          <t>SW238224</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>DBSS0909</t>
+          <t>M31-1200-45505</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Douchebak 90x90cm Vierkant SMC Hoogglans Wit</t>
+          <t>Badkamerspiegel met Verlichting 120x60cm</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1332,39 +1332,39 @@
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>douches</t>
+          <t>badkamerspiegels</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>douchebakken</t>
+          <t>badkamerspiegels-met-verlichting</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>139</v>
+        <v>169</v>
       </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-90x90cm-vierkant-smc-hoogglans-wit-13105/</t>
+          <t>https://www.maxaro.nl/badkamerspiegels/badkamerspiegels-met-verlichting/badkamerspiegel-met-verlichting-120x60cm-6524/</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>SW238224</t>
+          <t>SW238201</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>M31-1200-45505</t>
+          <t>DBSS0909</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Badkamerspiegel met Verlichting 120x60cm</t>
+          <t>Douchebak 90x90cm Vierkant SMC Hoogglans Wit</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1375,39 +1375,39 @@
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>badkamerspiegels</t>
+          <t>douches</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>badkamerspiegels-met-verlichting</t>
+          <t>douchebakken</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/badkamerspiegels/badkamerspiegels-met-verlichting/badkamerspiegel-met-verlichting-120x60cm-6524/</t>
+          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-90x90cm-vierkant-smc-hoogglans-wit-13105/</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>SW358008</t>
+          <t>SW238222</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>200-1202MB</t>
+          <t>EC-0909013</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>WC Borstel Radius Black, Hangend, Zwart</t>
+          <t>Douchecabine Zircon Essence Helder 90x90cm Vierkant met Draaideur</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1418,39 +1418,39 @@
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>badkameraccessoires</t>
+          <t>douches</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>wc-borstels</t>
+          <t>douchecabines</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>47.95</v>
+        <v>319</v>
       </c>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/badkameraccessoires/wc-borstels/wc-borstel-radius-black-hangend-zwart-13223/</t>
+          <t>https://www.maxaro.nl/douches/douchecabines/douchecabine-zircon-essence-helder-90x90cm-vierkant-met-draaideur-80992/</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>SW2328</t>
+          <t>SW358008</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>IPA12300M</t>
+          <t>200-1202MB</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 120cm Veiligheidsglas 8mm Mat Zwart</t>
+          <t>WC Borstel Radius Black, Hangend, Zwart</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1461,39 +1461,39 @@
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>douches</t>
+          <t>badkameraccessoires</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>inloopdouches</t>
+          <t>wc-borstels</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>340</v>
+        <v>47.95</v>
       </c>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-120cm-veiligheidsglas-8mm-mat-zwart-11185/</t>
+          <t>https://www.maxaro.nl/badkameraccessoires/wc-borstels/wc-borstel-radius-black-hangend-zwart-13223/</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>SW238222</t>
+          <t>SW238231</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>EC-0909013</t>
+          <t>GW-08013</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Douchecabine Zircon Essence Helder 90x90cm Vierkant met Draaideur</t>
+          <t>Douchewand Inloopdouche 80cm Veiligheidsglas 6 mm Chroom</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1509,34 +1509,34 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>douchecabines</t>
+          <t>inloopdouches</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>319</v>
+        <v>140</v>
       </c>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchecabines/douchecabine-zircon-essence-helder-90x90cm-vierkant-met-draaideur-80992/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-80cm-veiligheidsglas-6-mm-chroom-81033/</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>SW238231</t>
+          <t>SW238205</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>GW-08013</t>
+          <t>150-1103MB</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 80cm Veiligheidsglas 6 mm Chroom</t>
+          <t>Toiletrolhouder Radius Black, Zwart</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1547,39 +1547,39 @@
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>douches</t>
+          <t>badkameraccessoires</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>inloopdouches</t>
+          <t>toiletrolhouders</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>140</v>
+        <v>27.95</v>
       </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-80cm-veiligheidsglas-6-mm-chroom-81033/</t>
+          <t>https://www.maxaro.nl/badkameraccessoires/toiletrolhouders/toiletrolhouder-radius-black-zwart-13244/</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>SW238205</t>
+          <t>SW209323</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>150-1103MB</t>
+          <t>S0411-0900N</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Toiletrolhouder Radius Black, Zwart</t>
+          <t>Douchedeur Zircon Comfort 90cm</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1590,39 +1590,39 @@
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
-          <t>badkameraccessoires</t>
+          <t>douches</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>toiletrolhouders</t>
+          <t>douchedeuren</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>27.95</v>
+        <v>285</v>
       </c>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/badkameraccessoires/toiletrolhouders/toiletrolhouder-radius-black-zwart-13244/</t>
+          <t>https://www.maxaro.nl/douches/douchedeuren/douchedeur-zircon-comfort-90cm-12575/</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SW209331</t>
+          <t>SW2328</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>IPA14305M</t>
+          <t>IPA12300M</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 140cm Zwarte Strepen Veiligheidsglas 8mm Mat Zwart</t>
+          <t>Douchewand Inloopdouche 120cm Veiligheidsglas 8mm Mat Zwart</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1642,30 +1642,30 @@
         </is>
       </c>
       <c r="I28" t="n">
-        <v>445</v>
+        <v>340</v>
       </c>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-140cm-zwarte-strepen-veiligheidsglas-8mm-mat-zwart-11219/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-120cm-veiligheidsglas-8mm-mat-zwart-11185/</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>SW209323</t>
+          <t>SW209331</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>S0411-0900N</t>
+          <t>IPA14305M</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Douchedeur Zircon Comfort 90cm</t>
+          <t>Douchewand Inloopdouche 140cm Zwarte Strepen Veiligheidsglas 8mm Mat Zwart</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1681,34 +1681,34 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>douchedeuren</t>
+          <t>inloopdouches</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>285</v>
+        <v>445</v>
       </c>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchedeuren/douchedeur-zircon-comfort-90cm-12575/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-140cm-zwarte-strepen-veiligheidsglas-8mm-mat-zwart-11219/</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SW238220</t>
+          <t>SW208812</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>M32-1200-45505</t>
+          <t>M31-0800-45505</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Badkamerspiegel met Verlichting Meso 120x60cm</t>
+          <t>Badkamerspiegel met Verlichting 80x60cm</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1728,30 +1728,30 @@
         </is>
       </c>
       <c r="I30" t="n">
-        <v>209</v>
+        <v>129</v>
       </c>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/badkamerspiegels/badkamerspiegels-met-verlichting/badkamerspiegel-met-verlichting-meso-120x60cm-6534/</t>
+          <t>https://www.maxaro.nl/badkamerspiegels/badkamerspiegels-met-verlichting/badkamerspiegel-met-verlichting-80x60cm-6517/</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>SW208812</t>
+          <t>SW238221</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>M31-0800-45505</t>
+          <t>L2805-0909C</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Badkamerspiegel met Verlichting 80x60cm</t>
+          <t>Douchecabine Ruby Essence Helder 90x90cm Vierkant met Schuifdeuren</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1762,21 +1762,21 @@
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
-          <t>badkamerspiegels</t>
+          <t>douches</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>badkamerspiegels-met-verlichting</t>
+          <t>douchecabines</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>129</v>
+        <v>199</v>
       </c>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/badkamerspiegels/badkamerspiegels-met-verlichting/badkamerspiegel-met-verlichting-80x60cm-6517/</t>
+          <t>https://www.maxaro.nl/douches/douchecabines/douchecabine-ruby-essence-helder-90x90cm-vierkant-met-schuifdeuren-12273/</t>
         </is>
       </c>
     </row>
@@ -1826,18 +1826,18 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>SW1211</t>
+          <t>SW238220</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>IPA08305M</t>
+          <t>M32-1200-45505</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 80cm Zwarte Strepen Veiligheidsglas 8mm Mat Zwart</t>
+          <t>Badkamerspiegel met Verlichting Meso 120x60cm</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1848,39 +1848,39 @@
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
-          <t>douches</t>
+          <t>badkamerspiegels</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>inloopdouches</t>
+          <t>badkamerspiegels-met-verlichting</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>375</v>
+        <v>209</v>
       </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-80cm-zwarte-strepen-veiligheidsglas-8mm-mat-zwart-11097/</t>
+          <t>https://www.maxaro.nl/badkamerspiegels/badkamerspiegels-met-verlichting/badkamerspiegel-met-verlichting-meso-120x60cm-6534/</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>SW238221</t>
+          <t>SW1211</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>L2805-0909C</t>
+          <t>IPA08305M</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Douchecabine Ruby Essence Helder 90x90cm Vierkant met Schuifdeuren</t>
+          <t>Douchewand Inloopdouche 80cm Zwarte Strepen Veiligheidsglas 8mm Mat Zwart</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1896,34 +1896,34 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>douchecabines</t>
+          <t>inloopdouches</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>199</v>
+        <v>375</v>
       </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchecabines/douchecabine-ruby-essence-helder-90x90cm-vierkant-met-schuifdeuren-12273/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-80cm-zwarte-strepen-veiligheidsglas-8mm-mat-zwart-11097/</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>SW238200</t>
+          <t>SW20529</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>R2805-0909C</t>
+          <t>109105Z</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Douchecabine Ruby Essence 90x90cm Kwartrond met Schuifdeuren</t>
+          <t>Douchewisser, Hangend, Glasbevestiging, Zwart</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1934,39 +1934,39 @@
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
-          <t>douches</t>
+          <t>badkameraccessoires</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>douchecabines</t>
+          <t>douchewissers</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>199</v>
+        <v>29.95</v>
       </c>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchecabines/douchecabine-ruby-essence-90x90cm-kwartrond-met-schuifdeuren-12389/</t>
+          <t>https://www.maxaro.nl/badkameraccessoires/douchewissers/douchewisser-hangend-glasbevestiging-zwart-13320/</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>SW237319</t>
+          <t>SW238200</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>S2805-1200C</t>
+          <t>R2805-0909C</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Douchewand met Schuifdeur Ruby Essence 120cm Chroom</t>
+          <t>Douchecabine Ruby Essence 90x90cm Kwartrond met Schuifdeuren</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1982,34 +1982,34 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>douchedeuren</t>
+          <t>douchecabines</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchedeuren/douchewand-met-schuifdeur-ruby-essence-120cm-chroom-12636/</t>
+          <t>https://www.maxaro.nl/douches/douchecabines/douchecabine-ruby-essence-90x90cm-kwartrond-met-schuifdeuren-12389/</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>SW238229</t>
+          <t>SW238213</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>XZ03-1775G</t>
+          <t>GW-07013</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Ligbad Capri 170x75cm Acryl Glans Wit</t>
+          <t>Douchewand Inloopdouche 70cm Veiligheidsglas 6 mm Chroom</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -2020,39 +2020,39 @@
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>baden</t>
+          <t>douches</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>ligbaden</t>
+          <t>inloopdouches</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>219</v>
+        <v>130</v>
       </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/baden/ligbaden/ligbad-capri-170x75cm-acryl-glans-wit-6655/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-70cm-veiligheidsglas-6-mm-chroom-81032/</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>SW1208</t>
+          <t>SW237319</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>L0820-0909C</t>
+          <t>S2805-1200C</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Douchecabine Ruby Allure Helder 90x90cm Vierkant met Schuifdeuren</t>
+          <t>Douchewand met Schuifdeur Ruby Essence 120cm Chroom</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -2068,34 +2068,34 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>douchecabines</t>
+          <t>douchedeuren</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>309</v>
+        <v>215</v>
       </c>
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchecabines/douchecabine-ruby-allure-helder-90x90cm-vierkant-met-schuifdeuren-12206/</t>
+          <t>https://www.maxaro.nl/douches/douchedeuren/douchewand-met-schuifdeur-ruby-essence-120cm-chroom-12636/</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>SW377841</t>
+          <t>SW238229</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>IPA12305M</t>
+          <t>XZ03-1775G</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 120cm Zwarte Strepen Veiligheidsglas 8mm Mat Zwart</t>
+          <t>Ligbad Capri 170x75cm Acryl Glans Wit</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -2106,39 +2106,39 @@
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr">
         <is>
-          <t>douches</t>
+          <t>baden</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>inloopdouches</t>
+          <t>ligbaden</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>425</v>
+        <v>219</v>
       </c>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-120cm-zwarte-strepen-veiligheidsglas-8mm-mat-zwart-11190/</t>
+          <t>https://www.maxaro.nl/baden/ligbaden/ligbad-capri-170x75cm-acryl-glans-wit-6655/</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>SW20529</t>
+          <t>SW1208</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>109105Z</t>
+          <t>L0820-0909C</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Douchewisser, Hangend, Glasbevestiging, Zwart</t>
+          <t>Douchecabine Ruby Allure Helder 90x90cm Vierkant met Schuifdeuren</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -2149,21 +2149,21 @@
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
-          <t>badkameraccessoires</t>
+          <t>douches</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>douchewissers</t>
+          <t>douchecabines</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>29.95</v>
+        <v>309</v>
       </c>
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/badkameraccessoires/douchewissers/douchewisser-hangend-glasbevestiging-zwart-13320/</t>
+          <t>https://www.maxaro.nl/douches/douchecabines/douchecabine-ruby-allure-helder-90x90cm-vierkant-met-schuifdeuren-12206/</t>
         </is>
       </c>
     </row>
@@ -2213,18 +2213,18 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>SW238213</t>
+          <t>SW377841</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>GW-07013</t>
+          <t>IPA12305M</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 70cm Veiligheidsglas 6 mm Chroom</t>
+          <t>Douchewand Inloopdouche 120cm Zwarte Strepen Veiligheidsglas 8mm Mat Zwart</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -2244,12 +2244,12 @@
         </is>
       </c>
       <c r="I42" t="n">
-        <v>130</v>
+        <v>425</v>
       </c>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-70cm-veiligheidsglas-6-mm-chroom-81032/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-120cm-zwarte-strepen-veiligheidsglas-8mm-mat-zwart-11190/</t>
         </is>
       </c>
     </row>
@@ -2299,18 +2299,18 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>SW208805</t>
+          <t>SW208803</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>M31-0600-65505</t>
+          <t>S0820-1300C</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Badkamerspiegel met Verlichting 60x80cm</t>
+          <t>Douchewand met Schuifdeur Ruby Allure 130cm Chroom</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2321,39 +2321,39 @@
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
-          <t>badkamerspiegels</t>
+          <t>douches</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>badkamerspiegels-met-verlichting</t>
+          <t>douchedeuren</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>129</v>
+        <v>334</v>
       </c>
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/badkamerspiegels/badkamerspiegels-met-verlichting/badkamerspiegel-met-verlichting-60x80cm-6516/</t>
+          <t>https://www.maxaro.nl/douches/douchedeuren/douchewand-met-schuifdeur-ruby-allure-130cm-chroom-12614/</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>SW208803</t>
+          <t>SW238198</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>S0820-1300C</t>
+          <t>S0310-0970N</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Douchewand met Schuifdeur Ruby Allure 130cm Chroom</t>
+          <t>Douchedeur 90cm Draaideur Zircon Comfort</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -2373,30 +2373,30 @@
         </is>
       </c>
       <c r="I45" t="n">
-        <v>334</v>
+        <v>255</v>
       </c>
       <c r="J45" t="inlineStr"/>
       <c r="K45" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchedeuren/douchewand-met-schuifdeur-ruby-allure-130cm-chroom-12614/</t>
+          <t>https://www.maxaro.nl/douches/douchedeuren/douchedeur-90cm-draaideur-zircon-comfort-12421/</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>SW238227</t>
+          <t>SW208805</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>IPA14300C</t>
+          <t>M31-0600-65505</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 140cm Veiligheidsglas 8mm Chroom</t>
+          <t>Badkamerspiegel met Verlichting 60x80cm</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -2407,39 +2407,39 @@
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr">
         <is>
-          <t>douches</t>
+          <t>badkamerspiegels</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>inloopdouches</t>
+          <t>badkamerspiegels-met-verlichting</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>305</v>
+        <v>129</v>
       </c>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-140cm-veiligheidsglas-8mm-chroom-11210/</t>
+          <t>https://www.maxaro.nl/badkamerspiegels/badkamerspiegels-met-verlichting/badkamerspiegel-met-verlichting-60x80cm-6516/</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>SW238196</t>
+          <t>SW238227</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>IPA12306C</t>
+          <t>IPA14300C</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 120cm Matte Strepen Veiligheidsglas 8mm Chroom</t>
+          <t>Douchewand Inloopdouche 140cm Veiligheidsglas 8mm Chroom</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -2459,30 +2459,30 @@
         </is>
       </c>
       <c r="I47" t="n">
-        <v>360</v>
+        <v>305</v>
       </c>
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-120cm-matte-strepen-veiligheidsglas-8mm-chroom-11191/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-140cm-veiligheidsglas-8mm-chroom-11210/</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>SW238198</t>
+          <t>SW238195</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>S0310-0970N</t>
+          <t>GW-05013</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Douchedeur 90cm Draaideur Zircon Comfort</t>
+          <t>Douchewand Inloopdouche 50cm Veiligheidsglas 6 mm Chroom</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -2498,16 +2498,16 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>douchedeuren</t>
+          <t>inloopdouches</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>255</v>
+        <v>110</v>
       </c>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchedeuren/douchedeur-90cm-draaideur-zircon-comfort-12421/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-50cm-veiligheidsglas-6-mm-chroom-81030/</t>
         </is>
       </c>
     </row>
@@ -2557,18 +2557,18 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>SW377810</t>
+          <t>SW238196</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>S0411-1000N</t>
+          <t>IPA12306C</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Douchedeur Zircon Comfort 100cm</t>
+          <t>Douchewand Inloopdouche 120cm Matte Strepen Veiligheidsglas 8mm Chroom</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -2584,16 +2584,16 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>douchedeuren</t>
+          <t>inloopdouches</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>299</v>
+        <v>360</v>
       </c>
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchedeuren/douchedeur-zircon-comfort-100cm-12576/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-120cm-matte-strepen-veiligheidsglas-8mm-chroom-11191/</t>
         </is>
       </c>
     </row>
@@ -2643,18 +2643,18 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>SW238195</t>
+          <t>SW208801</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>GW-05013</t>
+          <t>DBAS0808G</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 50cm Veiligheidsglas 6 mm Chroom</t>
+          <t>Douchebak 80x80cm Vierkant Acryl Hoogglans Wit</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -2670,34 +2670,34 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>inloopdouches</t>
+          <t>douchebakken</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J52" t="inlineStr"/>
       <c r="K52" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-50cm-veiligheidsglas-6-mm-chroom-81030/</t>
+          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-80x80cm-vierkant-acryl-hoogglans-wit-13078/</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>SW23918</t>
+          <t>SW23913</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>IQA12300C</t>
+          <t>IPA14305M</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche Quartz 120cm Veiligheidsglas 8mm Chroom</t>
+          <t>Douchewand Inloopdouche 140cm Zwarte Strepen Veiligheidsglas 8mm Mat Zwart</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -2717,30 +2717,30 @@
         </is>
       </c>
       <c r="I53" t="n">
-        <v>320</v>
+        <v>445</v>
       </c>
       <c r="J53" t="inlineStr"/>
       <c r="K53" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-quartz-120cm-veiligheidsglas-8mm-chroom-12007/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-140cm-zwarte-strepen-veiligheidsglas-8mm-mat-zwart-11219/</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>SW23913</t>
+          <t>SW23918</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>IPA14305M</t>
+          <t>IQA12300C</t>
         </is>
       </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 140cm Zwarte Strepen Veiligheidsglas 8mm Mat Zwart</t>
+          <t>Douchewand Inloopdouche Quartz 120cm Veiligheidsglas 8mm Chroom</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -2760,12 +2760,12 @@
         </is>
       </c>
       <c r="I54" t="n">
-        <v>445</v>
+        <v>320</v>
       </c>
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-140cm-zwarte-strepen-veiligheidsglas-8mm-mat-zwart-11219/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-quartz-120cm-veiligheidsglas-8mm-chroom-12007/</t>
         </is>
       </c>
     </row>
@@ -2858,18 +2858,18 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>SW88209</t>
+          <t>SW377810</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>IPA10306C</t>
+          <t>S0411-1000N</t>
         </is>
       </c>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 100cm Matte Strepen Veiligheidsglas 8mm Chroom</t>
+          <t>Douchedeur Zircon Comfort 100cm</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -2885,34 +2885,34 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>inloopdouches</t>
+          <t>douchedeuren</t>
         </is>
       </c>
       <c r="I57" t="n">
-        <v>340</v>
+        <v>299</v>
       </c>
       <c r="J57" t="inlineStr"/>
       <c r="K57" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-100cm-matte-strepen-veiligheidsglas-8mm-chroom-11158/</t>
+          <t>https://www.maxaro.nl/douches/douchedeuren/douchedeur-zircon-comfort-100cm-12576/</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>SW208801</t>
+          <t>SW208813</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>DBAS0808G</t>
+          <t>GW-04013</t>
         </is>
       </c>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Douchebak 80x80cm Vierkant Acryl Hoogglans Wit</t>
+          <t>Douchewand Inloopdouche 40cm Veiligheidsglas 6 mm Chroom</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2928,34 +2928,34 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>douchebakken</t>
+          <t>inloopdouches</t>
         </is>
       </c>
       <c r="I58" t="n">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="J58" t="inlineStr"/>
       <c r="K58" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-80x80cm-vierkant-acryl-hoogglans-wit-13078/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-40cm-veiligheidsglas-6-mm-chroom-81029/</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>SW208813</t>
+          <t>SW238217</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>GW-04013</t>
+          <t>M32-0600-55505</t>
         </is>
       </c>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 40cm Veiligheidsglas 6 mm Chroom</t>
+          <t>Badkamerspiegel met Verlichting 60x70cm</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2966,39 +2966,39 @@
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr">
         <is>
-          <t>douches</t>
+          <t>badkamerspiegels</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>inloopdouches</t>
+          <t>badkamerspiegels-met-verlichting</t>
         </is>
       </c>
       <c r="I59" t="n">
-        <v>100</v>
+        <v>159</v>
       </c>
       <c r="J59" t="inlineStr"/>
       <c r="K59" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-40cm-veiligheidsglas-6-mm-chroom-81029/</t>
+          <t>https://www.maxaro.nl/badkamerspiegels/badkamerspiegels-met-verlichting/badkamerspiegel-met-verlichting-60x70cm-6528/</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>SW238217</t>
+          <t>SW238216</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>M32-0600-55505</t>
+          <t>DBAR1009G</t>
         </is>
       </c>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Badkamerspiegel met Verlichting 60x70cm</t>
+          <t>Douchebak 100x90cm Rechthoek Acryl Hoogglans Wit</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -3009,39 +3009,39 @@
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr">
         <is>
-          <t>badkamerspiegels</t>
+          <t>douches</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>badkamerspiegels-met-verlichting</t>
+          <t>douchebakken</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="J60" t="inlineStr"/>
       <c r="K60" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/badkamerspiegels/badkamerspiegels-met-verlichting/badkamerspiegel-met-verlichting-60x70cm-6528/</t>
+          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-100x90cm-rechthoek-acryl-hoogglans-wit-13053/</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>SW238216</t>
+          <t>SW208806</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>DBAR1009G</t>
+          <t>IPA14300M</t>
         </is>
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Douchebak 100x90cm Rechthoek Acryl Hoogglans Wit</t>
+          <t>Douchewand Inloopdouche 140cm Veiligheidsglas 8mm Mat Zwart</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -3057,34 +3057,34 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>douchebakken</t>
+          <t>inloopdouches</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>145</v>
+        <v>370</v>
       </c>
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-100x90cm-rechthoek-acryl-hoogglans-wit-13053/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-140cm-veiligheidsglas-8mm-mat-zwart-11211/</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>SW208806</t>
+          <t>SW238199</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>IPA14300M</t>
+          <t>DBSS1010</t>
         </is>
       </c>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Douchewand Inloopdouche 140cm Veiligheidsglas 8mm Mat Zwart</t>
+          <t>Douchebak 100x100cm Vierkant SMC Hoogglans Wit</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -3100,34 +3100,34 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>inloopdouches</t>
+          <t>douchebakken</t>
         </is>
       </c>
       <c r="I62" t="n">
-        <v>370</v>
+        <v>159</v>
       </c>
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-140cm-veiligheidsglas-8mm-mat-zwart-11211/</t>
+          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-100x100cm-vierkant-smc-hoogglans-wit-13106/</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>SW238194</t>
+          <t>SW209329</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>DBAS0808G</t>
+          <t>EC-0808011</t>
         </is>
       </c>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Douchebak 80x80cm Vierkant Acryl Hoogglans Wit</t>
+          <t>Douchecabine Zircon Essence Helder 80x80cm Vierkant met Draaideur</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -3143,34 +3143,34 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>douchebakken</t>
+          <t>douchecabines</t>
         </is>
       </c>
       <c r="I63" t="n">
-        <v>105</v>
+        <v>304</v>
       </c>
       <c r="J63" t="inlineStr"/>
       <c r="K63" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-80x80cm-vierkant-acryl-hoogglans-wit-13078/</t>
+          <t>https://www.maxaro.nl/douches/douchecabines/douchecabine-zircon-essence-helder-80x80cm-vierkant-met-draaideur-10935/</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>SW208800</t>
+          <t>SW88209</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>DBAP1010G</t>
+          <t>IPA10306C</t>
         </is>
       </c>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Douchebak 100x100cm Vijfhoek Acryl Hoogglans Wit</t>
+          <t>Douchewand Inloopdouche 100cm Matte Strepen Veiligheidsglas 8mm Chroom</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -3186,34 +3186,34 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>douchebakken</t>
+          <t>inloopdouches</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>145</v>
+        <v>340</v>
       </c>
       <c r="J64" t="inlineStr"/>
       <c r="K64" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-100x100cm-vijfhoek-acryl-hoogglans-wit-13048/</t>
+          <t>https://www.maxaro.nl/douches/inloopdouches/douchewand-inloopdouche-100cm-matte-strepen-veiligheidsglas-8mm-chroom-11158/</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>SW238199</t>
+          <t>SW238194</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>DBSS1010</t>
+          <t>DBAS0808G</t>
         </is>
       </c>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Douchebak 100x100cm Vierkant SMC Hoogglans Wit</t>
+          <t>Douchebak 80x80cm Vierkant Acryl Hoogglans Wit</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -3233,30 +3233,30 @@
         </is>
       </c>
       <c r="I65" t="n">
-        <v>159</v>
+        <v>105</v>
       </c>
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-100x100cm-vierkant-smc-hoogglans-wit-13106/</t>
+          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-80x80cm-vierkant-acryl-hoogglans-wit-13078/</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>SW209329</t>
+          <t>SW2104</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>EC-0808011</t>
+          <t>DBAS0909G</t>
         </is>
       </c>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Douchecabine Zircon Essence Helder 80x80cm Vierkant met Draaideur</t>
+          <t>Douchebak 90x90cm Vierkant Acryl Hoogglans Wit</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -3272,34 +3272,34 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>douchecabines</t>
+          <t>douchebakken</t>
         </is>
       </c>
       <c r="I66" t="n">
-        <v>304</v>
+        <v>115</v>
       </c>
       <c r="J66" t="inlineStr"/>
       <c r="K66" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchecabines/douchecabine-zircon-essence-helder-80x80cm-vierkant-met-draaideur-10935/</t>
+          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-90x90cm-vierkant-acryl-hoogglans-wit-13079/</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>SW2104</t>
+          <t>SW208800</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>DBAS0909G</t>
+          <t>DBAP1010G</t>
         </is>
       </c>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Douchebak 90x90cm Vierkant Acryl Hoogglans Wit</t>
+          <t>Douchebak 100x100cm Vijfhoek Acryl Hoogglans Wit</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -3319,12 +3319,12 @@
         </is>
       </c>
       <c r="I67" t="n">
-        <v>115</v>
+        <v>145</v>
       </c>
       <c r="J67" t="inlineStr"/>
       <c r="K67" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-90x90cm-vierkant-acryl-hoogglans-wit-13079/</t>
+          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-100x100cm-vijfhoek-acryl-hoogglans-wit-13048/</t>
         </is>
       </c>
     </row>
@@ -3374,18 +3374,18 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>SW2108</t>
+          <t>SW238215</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>DBSQ0808</t>
+          <t>DBAP0909G</t>
         </is>
       </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Douchebak 80x80cm Kwartrond SMC Hoogglans Wit</t>
+          <t>Douchebak 90x90cm Vijfhoek Acryl Hoogglans Wit</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -3405,30 +3405,30 @@
         </is>
       </c>
       <c r="I69" t="n">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="J69" t="inlineStr"/>
       <c r="K69" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-80x80cm-kwartrond-smc-hoogglans-wit-13090/</t>
+          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-90x90cm-vijfhoek-acryl-hoogglans-wit-13047/</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>SW238215</t>
+          <t>SW2108</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>DBAP0909G</t>
+          <t>DBSQ0808</t>
         </is>
       </c>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Douchebak 90x90cm Vijfhoek Acryl Hoogglans Wit</t>
+          <t>Douchebak 80x80cm Kwartrond SMC Hoogglans Wit</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -3448,30 +3448,30 @@
         </is>
       </c>
       <c r="I70" t="n">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-90x90cm-vijfhoek-acryl-hoogglans-wit-13047/</t>
+          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-80x80cm-kwartrond-smc-hoogglans-wit-13090/</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>SW238230</t>
+          <t>SW23916</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>DBAQ0909G</t>
+          <t>DBAS1010G</t>
         </is>
       </c>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Douchebak 90x90cm Kwartrond Acryl Hoogglans Wit</t>
+          <t>Douchebak 100x100cm Vierkant Acryl Hoogglans Wit</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -3491,30 +3491,30 @@
         </is>
       </c>
       <c r="I71" t="n">
-        <v>109</v>
+        <v>149</v>
       </c>
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-90x90cm-kwartrond-acryl-hoogglans-wit-13050/</t>
+          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-100x100cm-vierkant-acryl-hoogglans-wit-13081/</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>SW23916</t>
+          <t>SW238230</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>DBAS1010G</t>
+          <t>DBAQ0909G</t>
         </is>
       </c>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Douchebak 100x100cm Vierkant Acryl Hoogglans Wit</t>
+          <t>Douchebak 90x90cm Kwartrond Acryl Hoogglans Wit</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -3534,30 +3534,30 @@
         </is>
       </c>
       <c r="I72" t="n">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-100x100cm-vierkant-acryl-hoogglans-wit-13081/</t>
+          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-90x90cm-kwartrond-acryl-hoogglans-wit-13050/</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>SW20840</t>
+          <t>SW377833</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>DBAQ0808G</t>
+          <t>DBAQ1010G</t>
         </is>
       </c>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Douchebak 80x80cm Kwartrond Acryl Hoogglans Wit</t>
+          <t>Douchebak 100x100cm Kwartrond Acryl Hoogglans Wit</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -3577,30 +3577,30 @@
         </is>
       </c>
       <c r="I73" t="n">
-        <v>99</v>
+        <v>149</v>
       </c>
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-80x80cm-kwartrond-acryl-hoogglans-wit-13049/</t>
+          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-100x100cm-kwartrond-acryl-hoogglans-wit-13051/</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>SW377833</t>
+          <t>SW20840</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>DBAQ1010G</t>
+          <t>DBAQ0808G</t>
         </is>
       </c>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Douchebak 100x100cm Kwartrond Acryl Hoogglans Wit</t>
+          <t>Douchebak 80x80cm Kwartrond Acryl Hoogglans Wit</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -3620,30 +3620,30 @@
         </is>
       </c>
       <c r="I74" t="n">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-100x100cm-kwartrond-acryl-hoogglans-wit-13051/</t>
+          <t>https://www.maxaro.nl/douches/douchebakken/douchebak-80x80cm-kwartrond-acryl-hoogglans-wit-13049/</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>SW377837</t>
+          <t>SW213536</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>M120-0041N</t>
+          <t>VSB11-MN</t>
         </is>
       </c>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Waskom Mintra Solid Surface Mat Wit 55x32,5cm Ovaal</t>
+          <t>Vrijstaand Bad Solid Surface Tesino 180x85cm Mat Wit</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -3654,39 +3654,39 @@
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr">
         <is>
-          <t>wastafels</t>
+          <t>baden</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>waskommen</t>
+          <t>vrijstaande-baden</t>
         </is>
       </c>
       <c r="I75" t="n">
-        <v>229</v>
+        <v>1995</v>
       </c>
       <c r="J75" t="inlineStr"/>
       <c r="K75" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/wastafels/waskommen/waskom-mintra-solid-surface-mat-wit-55x325cm-ovaal-7206/</t>
+          <t>https://www.maxaro.nl/baden/vrijstaande-baden/vrijstaand-bad-solid-surface-tesino-180x85cm-mat-wit-6714/</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>SW213536</t>
+          <t>SW377837</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>VSB11-MN</t>
+          <t>M120-0041N</t>
         </is>
       </c>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Vrijstaand Bad Solid Surface Tesino 180x85cm Mat Wit</t>
+          <t>Waskom Mintra Solid Surface Mat Wit 55x32,5cm Ovaal</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -3697,21 +3697,21 @@
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr">
         <is>
-          <t>baden</t>
+          <t>wastafels</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>vrijstaande-baden</t>
+          <t>waskommen</t>
         </is>
       </c>
       <c r="I76" t="n">
-        <v>1995</v>
+        <v>229</v>
       </c>
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr">
         <is>
-          <t>https://www.maxaro.nl/baden/vrijstaande-baden/vrijstaand-bad-solid-surface-tesino-180x85cm-mat-wit-6714/</t>
+          <t>https://www.maxaro.nl/wastafels/waskommen/waskom-mintra-solid-surface-mat-wit-55x325cm-ovaal-7206/</t>
         </is>
       </c>
     </row>

</xml_diff>